<commit_message>
changed DataCapture readme to be up to date. Cleaned up some formatting of Read_IMU_And_LeapDevice.m
</commit_message>
<xml_diff>
--- a/DataCapture/GUID_Directory.xlsx
+++ b/DataCapture/GUID_Directory.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>000309</t>
   </si>
@@ -31,6 +31,12 @@
   </si>
   <si>
     <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 24-Mar-2023 12:36:53</t>
+  </si>
+  <si>
+    <t>000312</t>
+  </si>
+  <si>
+    <t>Details: Palm Position and Baton tip position - transformed IMU CJMCU-20948 Data Reading and single hand Leap LM-010 Reading. Script used: Read_IMU_And_LeapDevice.  Dataset used: Live test data from raw imu reading and raw leap reading. baton length of 50 - transforming along z axis now.. File Location: Visualisations/IMU_Leap_CombinedData. Date Generated: 24-Mar-2023 14:04:17</t>
   </si>
 </sst>
 </file>
@@ -76,7 +82,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.140625" customWidth="true"/>
@@ -107,6 +113,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>